<commit_message>
Inputs using gradients of protein content and cytokinins content
</commit_message>
<xml_diff>
--- a/branches/develop/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/develop/fspmwheat/inputs/Generate_inputs.xlsx
@@ -12,10 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="INPUTS" sheetId="1" r:id="rId1"/>
     <sheet name="N content" sheetId="2" r:id="rId2"/>
     <sheet name="Conc Shoot" sheetId="3" r:id="rId3"/>
     <sheet name="N crit" sheetId="4" r:id="rId4"/>
+    <sheet name="Barillot2016b_inputs" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="204">
   <si>
     <t>plant</t>
   </si>
@@ -661,6 +662,96 @@
   <si>
     <t>N crit</t>
   </si>
+  <si>
+    <t>Input Barillot 2016b</t>
+  </si>
+  <si>
+    <t>cm2</t>
+  </si>
+  <si>
+    <t>g m-2</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>AU.g-1</t>
+  </si>
+  <si>
+    <t>Phyto</t>
+  </si>
+  <si>
+    <t>Organ</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>SSW</t>
+  </si>
+  <si>
+    <t>cyto</t>
+  </si>
+  <si>
+    <t>conc_cyto</t>
+  </si>
+  <si>
+    <t>IN_exp</t>
+  </si>
+  <si>
+    <t>IN_enc</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>Roots</t>
+  </si>
+  <si>
+    <t>Manip PostDoc Romain : dosage N précoce</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>2 feuilles ligulees + 2 en croissance</t>
+  </si>
+  <si>
+    <t>Étiquettes de lignes</t>
+  </si>
+  <si>
+    <t>Moyenne de N [%]</t>
+  </si>
+  <si>
+    <t>Écartype de N [%]</t>
+  </si>
+  <si>
+    <t>Gaine</t>
+  </si>
+  <si>
+    <t>Graines</t>
+  </si>
+  <si>
+    <t>Limbe</t>
+  </si>
+  <si>
+    <t>ENC</t>
+  </si>
+  <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>Densité semis</t>
+  </si>
+  <si>
+    <t>170 pl.m-2</t>
+  </si>
+  <si>
+    <t>%N</t>
+  </si>
 </sst>
 </file>
 
@@ -669,7 +760,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -770,6 +861,22 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -965,7 +1072,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -997,13 +1104,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1019,9 +1123,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1036,12 +1137,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,6 +1164,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>674483</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>109655</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3362325" y="13134975"/>
+          <a:ext cx="5694158" cy="3548180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1322,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT44"/>
+  <dimension ref="A1:AV44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="U37" sqref="U37"/>
+    <sheetView tabSelected="1" topLeftCell="N12" workbookViewId="0">
+      <selection activeCell="AD37" sqref="AD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,20 +1483,20 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>34</v>
       </c>
       <c r="W1" s="7"/>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+    <row r="3" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1440,8 +1590,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A4" s="49"/>
       <c r="B4">
         <v>1</v>
       </c>
@@ -1533,8 +1683,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A5" s="49"/>
       <c r="B5">
         <v>1</v>
       </c>
@@ -1626,8 +1776,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A6" s="49"/>
       <c r="B6">
         <v>1</v>
       </c>
@@ -1719,8 +1869,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
       <c r="B7">
         <v>1</v>
       </c>
@@ -1812,8 +1962,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -1905,8 +2055,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
       <c r="B9">
         <v>1</v>
       </c>
@@ -1998,8 +2148,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A10" s="49"/>
       <c r="B10">
         <v>1</v>
       </c>
@@ -2091,8 +2241,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
       <c r="B11">
         <v>1</v>
       </c>
@@ -2184,8 +2334,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
       <c r="B12">
         <v>1</v>
       </c>
@@ -2277,13 +2427,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:46" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:46" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+    <row r="16" spans="1:48" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="49" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -2397,28 +2547,37 @@
       <c r="AL16" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AN16" s="10" t="s">
+      <c r="AM16" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="AN16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO16" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP16" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="AO16" s="10" t="s">
+      <c r="AQ16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="AP16" s="10" t="s">
+      <c r="AR16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AQ16" s="10" t="s">
+      <c r="AS16" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="AR16" s="10" t="s">
+      <c r="AT16" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="AS16" s="10"/>
-      <c r="AT16" s="10" t="s">
+      <c r="AU16" s="10"/>
+      <c r="AV16" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A17" s="49"/>
       <c r="B17">
         <v>1</v>
       </c>
@@ -2504,26 +2663,26 @@
         <v>33</v>
       </c>
       <c r="AC17" s="1">
-        <f t="shared" ref="AC17:AC24" si="0">AI17*$Z$28</f>
+        <f t="shared" ref="AC17:AC24" si="0">AI17*$AA$28</f>
         <v>4.4515747404911092</v>
       </c>
-      <c r="AD17">
-        <f t="shared" ref="AD17:AD24" si="1">AI17*$U$28</f>
-        <v>0.54148939294380627</v>
+      <c r="AD17" s="1">
+        <f>AI17*$AN17</f>
+        <v>0.56052414587208832</v>
       </c>
       <c r="AE17">
         <v>0</v>
       </c>
-      <c r="AF17">
-        <f t="shared" ref="AF17:AF24" si="2">AI17*$V$28</f>
-        <v>7.7355627563400891</v>
+      <c r="AF17" s="1">
+        <f>AI17*$AO17</f>
+        <v>8.00748779817269</v>
       </c>
       <c r="AG17" s="1">
-        <f>AQ17</f>
+        <f>AS17</f>
         <v>1.8534983222633695E-3</v>
       </c>
       <c r="AH17" s="1">
-        <f>AT17</f>
+        <f>AV17</f>
         <v>1.3244862745926676E-6</v>
       </c>
       <c r="AI17" s="1">
@@ -2542,33 +2701,44 @@
         <f>AJ17+AK17</f>
         <v>9.2741140426898098E-6</v>
       </c>
-      <c r="AN17" s="11">
+      <c r="AM17" s="17">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AN17" s="17">
+        <f>(($AM17/100)*(1+$AA$28*$E$43)-$X$28)/(((1+1/$W$35)*(14*10^(-6)))-(($J$43/$W$35+$F$43)*$AM17/100))</f>
+        <v>302.19821715148822</v>
+      </c>
+      <c r="AO17" s="17">
+        <f>$AN17/$W$35</f>
+        <v>4317.117387878403</v>
+      </c>
+      <c r="AP17" s="11">
         <v>851425</v>
       </c>
-      <c r="AO17" s="12">
+      <c r="AQ17" s="12">
         <f>$T$39+$T$40*$T$42*(I17)^$T$41</f>
         <v>9.1058115591388438E-4</v>
       </c>
-      <c r="AP17" s="11">
-        <f t="shared" ref="AP17:AP24" si="3">I17*X17</f>
+      <c r="AR17" s="11">
+        <f t="shared" ref="AR17:AR24" si="1">I17*X17</f>
         <v>2.3159999999999999E-3</v>
       </c>
-      <c r="AQ17" s="12">
-        <f>((AP17-AO17)/($T$43-AN17))*(E17-$T$43)+AP17</f>
+      <c r="AS17" s="12">
+        <f>((AR17-AQ17)/($T$43-AP17))*(E17-$T$43)+AR17</f>
         <v>1.8534983222633695E-3</v>
       </c>
-      <c r="AR17" s="12">
-        <f t="shared" ref="AR17:AR24" si="4">$T$39+$T$40*$T$42*(K17)^$T$41</f>
+      <c r="AT17" s="12">
+        <f t="shared" ref="AT17:AT24" si="2">$T$39+$T$40*$T$42*(K17)^$T$41</f>
         <v>4.0277279389003447E-3</v>
       </c>
-      <c r="AS17" s="11"/>
-      <c r="AT17" s="11">
-        <f t="shared" ref="AT17:AT24" si="5">$AO$32*$AO$34*$AO$36*(L17)^$AO$33</f>
+      <c r="AU17" s="11"/>
+      <c r="AV17" s="11">
+        <f t="shared" ref="AV17:AV24" si="3">$AR$32*$AQ$34*$AQ$36*(L17)^$AQ$33</f>
         <v>1.3244862745926676E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A18" s="49"/>
       <c r="B18">
         <v>1</v>
       </c>
@@ -2595,7 +2765,7 @@
         <v>2.894E-2</v>
       </c>
       <c r="J18">
-        <f t="shared" ref="J18:J24" si="6">I18-L18</f>
+        <f t="shared" ref="J18:J24" si="4">I18-L18</f>
         <v>2.8930000000000001E-2</v>
       </c>
       <c r="K18">
@@ -2656,23 +2826,23 @@
         <f t="shared" si="0"/>
         <v>1.9049336424038494</v>
       </c>
-      <c r="AD18">
-        <f t="shared" si="1"/>
-        <v>0.23171606044060178</v>
+      <c r="AD18" s="1">
+        <f t="shared" ref="AD18:AD24" si="5">AI18*$AN18</f>
+        <v>0.35221208552901617</v>
       </c>
       <c r="AE18">
         <v>0</v>
       </c>
-      <c r="AF18">
-        <f t="shared" si="2"/>
-        <v>3.31022943486574</v>
+      <c r="AF18" s="1">
+        <f t="shared" ref="AF18:AF24" si="6">AI18*$AO18</f>
+        <v>5.0316012218430881</v>
       </c>
       <c r="AG18" s="1">
-        <f>AR18</f>
+        <f>AT18</f>
         <v>7.9355355356128927E-4</v>
       </c>
       <c r="AH18" s="1">
-        <f>AT18</f>
+        <f>AV18</f>
         <v>1.6879744031468265E-7</v>
       </c>
       <c r="AI18">
@@ -2691,33 +2861,44 @@
         <f t="shared" ref="AL18:AL24" si="9">AJ18+AK18</f>
         <v>3.9686117550080197E-6</v>
       </c>
-      <c r="AN18" s="11">
+      <c r="AM18" s="17">
+        <v>5.8</v>
+      </c>
+      <c r="AN18" s="17">
+        <f t="shared" ref="AN18:AN24" si="10">(($AM18/100)*(1+$AA$28*$E$43)-$X$28)/(((1+1/$W$35)*(14*10^(-6)))-(($J$43/$W$35+$F$43)*$AM18/100))</f>
+        <v>443.74721851357367</v>
+      </c>
+      <c r="AO18" s="17">
+        <f t="shared" ref="AO18:AO24" si="11">$AN18/$W$35</f>
+        <v>6339.2459787653379</v>
+      </c>
+      <c r="AP18" s="11">
         <v>818263</v>
       </c>
-      <c r="AO18" s="12">
+      <c r="AQ18" s="12">
         <f>$T$39+$T$40*$T$42*(I18)^$T$41</f>
         <v>9.1017858127080242E-4</v>
       </c>
-      <c r="AP18" s="11">
+      <c r="AR18" s="11">
+        <f t="shared" si="1"/>
+        <v>2.3151999999999999E-3</v>
+      </c>
+      <c r="AS18" s="12">
+        <f>((AR18-AQ18)/($T$43-AP18))*(E18-$T$43)+AR18</f>
+        <v>8.5826926811062858E-4</v>
+      </c>
+      <c r="AT18" s="12">
+        <f t="shared" si="2"/>
+        <v>7.9355355356128927E-4</v>
+      </c>
+      <c r="AU18" s="11"/>
+      <c r="AV18" s="11">
         <f t="shared" si="3"/>
-        <v>2.3151999999999999E-3</v>
-      </c>
-      <c r="AQ18" s="12">
-        <f>((AP18-AO18)/($T$43-AN18))*(E18-$T$43)+AP18</f>
-        <v>8.5826926811062858E-4</v>
-      </c>
-      <c r="AR18" s="12">
-        <f t="shared" si="4"/>
-        <v>7.9355355356128927E-4</v>
-      </c>
-      <c r="AS18" s="11"/>
-      <c r="AT18" s="11">
-        <f t="shared" si="5"/>
         <v>1.6879744031468265E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A19" s="49"/>
       <c r="B19">
         <v>1</v>
       </c>
@@ -2744,7 +2925,7 @@
         <v>2.894E-2</v>
       </c>
       <c r="J19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.894E-2</v>
       </c>
       <c r="K19">
@@ -2805,19 +2986,19 @@
         <f t="shared" si="0"/>
         <v>7.6004635065645101E-2</v>
       </c>
-      <c r="AD19">
-        <f t="shared" si="1"/>
-        <v>9.2452011033900532E-3</v>
+      <c r="AD19" s="1">
+        <f t="shared" si="5"/>
+        <v>1.492301535568265E-2</v>
       </c>
       <c r="AE19">
         <v>0</v>
       </c>
-      <c r="AF19">
-        <f t="shared" si="2"/>
-        <v>0.13207430147700075</v>
+      <c r="AF19" s="1">
+        <f t="shared" si="6"/>
+        <v>0.21318593365260927</v>
       </c>
       <c r="AG19" s="1">
-        <f>AR19</f>
+        <f>AT19</f>
         <v>3.1668597944018791E-5</v>
       </c>
       <c r="AH19" s="1">
@@ -2839,31 +3020,42 @@
         <f t="shared" si="9"/>
         <v>1.5834298972009396E-7</v>
       </c>
-      <c r="AN19" s="11"/>
-      <c r="AO19" s="12" t="e">
-        <f t="shared" ref="AO19:AO24" si="10">$T$39+$T$40*$T$42*(S19*$T$44)^$T$41</f>
+      <c r="AM19" s="17">
+        <v>6</v>
+      </c>
+      <c r="AN19" s="17">
+        <f t="shared" si="10"/>
+        <v>471.22437760150797</v>
+      </c>
+      <c r="AO19" s="17">
+        <f t="shared" si="11"/>
+        <v>6731.7768228786845</v>
+      </c>
+      <c r="AP19" s="11"/>
+      <c r="AQ19" s="12" t="e">
+        <f t="shared" ref="AQ19:AQ24" si="12">$T$39+$T$40*$T$42*(S19*$T$44)^$T$41</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AP19" s="11" t="e">
+      <c r="AR19" s="11" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS19" s="12" t="e">
+        <f t="shared" ref="AS19:AS24" si="13">AQ19+((AR19-AQ19)/$T$43)*E19</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT19" s="12">
+        <f t="shared" si="2"/>
+        <v>3.1668597944018791E-5</v>
+      </c>
+      <c r="AU19" s="11"/>
+      <c r="AV19" s="11">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AQ19" s="12" t="e">
-        <f t="shared" ref="AQ19:AQ24" si="11">AO19+((AP19-AO19)/$T$43)*E19</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AR19" s="12">
-        <f t="shared" si="4"/>
-        <v>3.1668597944018791E-5</v>
-      </c>
-      <c r="AS19" s="11"/>
-      <c r="AT19" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A20" s="49"/>
       <c r="B20">
         <v>1</v>
       </c>
@@ -2886,11 +3078,11 @@
         <v>33</v>
       </c>
       <c r="I20">
-        <f t="shared" ref="I20:I24" si="12">I19-L20</f>
+        <f t="shared" ref="I20:I24" si="14">I19-L20</f>
         <v>2.894E-2</v>
       </c>
       <c r="J20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.894E-2</v>
       </c>
       <c r="K20">
@@ -2951,19 +3143,19 @@
         <f t="shared" si="0"/>
         <v>1.347501240661572E-2</v>
       </c>
-      <c r="AD20">
-        <f t="shared" si="1"/>
-        <v>1.6391000293895159E-3</v>
+      <c r="AD20" s="1">
+        <f t="shared" si="5"/>
+        <v>2.6457309727000379E-3</v>
       </c>
       <c r="AE20">
         <v>0</v>
       </c>
-      <c r="AF20">
-        <f t="shared" si="2"/>
-        <v>2.341571470556451E-2</v>
+      <c r="AF20" s="1">
+        <f t="shared" si="6"/>
+        <v>3.7796156752857676E-2</v>
       </c>
       <c r="AG20" s="1">
-        <f t="shared" ref="AG20:AG24" si="13">AR20</f>
+        <f t="shared" ref="AG20:AG24" si="15">AT20</f>
         <v>5.6145885027565499E-6</v>
       </c>
       <c r="AH20" s="1">
@@ -2985,31 +3177,42 @@
         <f t="shared" si="9"/>
         <v>2.8072942513782751E-8</v>
       </c>
-      <c r="AN20" s="11"/>
-      <c r="AO20" s="12" t="e">
+      <c r="AM20" s="17">
+        <v>6</v>
+      </c>
+      <c r="AN20" s="17">
         <f t="shared" si="10"/>
+        <v>471.22437760150797</v>
+      </c>
+      <c r="AO20" s="17">
+        <f t="shared" si="11"/>
+        <v>6731.7768228786845</v>
+      </c>
+      <c r="AP20" s="11"/>
+      <c r="AQ20" s="12" t="e">
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AP20" s="11" t="e">
+      <c r="AR20" s="11" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS20" s="12" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT20" s="12">
+        <f t="shared" si="2"/>
+        <v>5.6145885027565499E-6</v>
+      </c>
+      <c r="AU20" s="11"/>
+      <c r="AV20" s="11">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AQ20" s="12" t="e">
-        <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AR20" s="12">
-        <f t="shared" si="4"/>
-        <v>5.6145885027565499E-6</v>
-      </c>
-      <c r="AS20" s="11"/>
-      <c r="AT20" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A21" s="49"/>
       <c r="B21">
         <v>1</v>
       </c>
@@ -3032,11 +3235,11 @@
         <v>33</v>
       </c>
       <c r="I21">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2.894E-2</v>
       </c>
       <c r="J21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.894E-2</v>
       </c>
       <c r="K21">
@@ -3097,19 +3300,19 @@
         <f t="shared" si="0"/>
         <v>4.4703594683963592E-3</v>
       </c>
-      <c r="AD21">
-        <f t="shared" si="1"/>
-        <v>5.4377436657740766E-4</v>
+      <c r="AD21" s="1">
+        <f t="shared" si="5"/>
+        <v>8.7772598256253436E-4</v>
       </c>
       <c r="AE21">
         <v>0</v>
       </c>
-      <c r="AF21">
-        <f t="shared" si="2"/>
-        <v>7.7682052368201098E-3</v>
+      <c r="AF21" s="1">
+        <f t="shared" si="6"/>
+        <v>1.2538942608036204E-2</v>
       </c>
       <c r="AG21" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.862649778498483E-6</v>
       </c>
       <c r="AH21" s="1">
@@ -3131,31 +3334,42 @@
         <f t="shared" si="9"/>
         <v>9.3132488924924148E-9</v>
       </c>
-      <c r="AN21" s="11"/>
-      <c r="AO21" s="12" t="e">
+      <c r="AM21" s="17">
+        <v>6</v>
+      </c>
+      <c r="AN21" s="17">
         <f t="shared" si="10"/>
+        <v>471.22437760150797</v>
+      </c>
+      <c r="AO21" s="17">
+        <f t="shared" si="11"/>
+        <v>6731.7768228786845</v>
+      </c>
+      <c r="AP21" s="11"/>
+      <c r="AQ21" s="12" t="e">
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AP21" s="11" t="e">
+      <c r="AR21" s="11" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS21" s="12" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT21" s="12">
+        <f t="shared" si="2"/>
+        <v>1.862649778498483E-6</v>
+      </c>
+      <c r="AU21" s="11"/>
+      <c r="AV21" s="11">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AQ21" s="12" t="e">
-        <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AR21" s="12">
-        <f t="shared" si="4"/>
-        <v>1.862649778498483E-6</v>
-      </c>
-      <c r="AS21" s="11"/>
-      <c r="AT21" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A22" s="49"/>
       <c r="B22">
         <v>1</v>
       </c>
@@ -3178,11 +3392,11 @@
         <v>33</v>
       </c>
       <c r="I22">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2.894E-2</v>
       </c>
       <c r="J22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.894E-2</v>
       </c>
       <c r="K22">
@@ -3243,19 +3457,19 @@
         <f t="shared" si="0"/>
         <v>1.8851448944099444E-3</v>
       </c>
-      <c r="AD22">
-        <f t="shared" si="1"/>
-        <v>2.2930895783916249E-4</v>
+      <c r="AD22" s="1">
+        <f t="shared" si="5"/>
+        <v>3.7013592898207774E-4</v>
       </c>
       <c r="AE22">
         <v>0</v>
       </c>
-      <c r="AF22">
-        <f t="shared" si="2"/>
-        <v>3.2758422548451785E-3</v>
+      <c r="AF22" s="1">
+        <f t="shared" si="6"/>
+        <v>5.2876561283153956E-3</v>
       </c>
       <c r="AG22" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>7.8547703933747685E-7</v>
       </c>
       <c r="AH22" s="1">
@@ -3277,31 +3491,42 @@
         <f t="shared" si="9"/>
         <v>3.9273851966873846E-9</v>
       </c>
-      <c r="AN22" s="11"/>
-      <c r="AO22" s="12" t="e">
+      <c r="AM22" s="17">
+        <v>6</v>
+      </c>
+      <c r="AN22" s="17">
         <f t="shared" si="10"/>
+        <v>471.22437760150797</v>
+      </c>
+      <c r="AO22" s="17">
+        <f t="shared" si="11"/>
+        <v>6731.7768228786845</v>
+      </c>
+      <c r="AP22" s="11"/>
+      <c r="AQ22" s="12" t="e">
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AP22" s="11" t="e">
+      <c r="AR22" s="11" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS22" s="12" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT22" s="12">
+        <f t="shared" si="2"/>
+        <v>7.8547703933747685E-7</v>
+      </c>
+      <c r="AU22" s="11"/>
+      <c r="AV22" s="11">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AQ22" s="12" t="e">
-        <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AR22" s="12">
-        <f t="shared" si="4"/>
-        <v>7.8547703933747685E-7</v>
-      </c>
-      <c r="AS22" s="11"/>
-      <c r="AT22" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A23" s="49"/>
       <c r="B23">
         <v>1</v>
       </c>
@@ -3324,11 +3549,11 @@
         <v>33</v>
       </c>
       <c r="I23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2.894E-2</v>
       </c>
       <c r="J23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.894E-2</v>
       </c>
       <c r="K23" s="1">
@@ -3389,19 +3614,19 @@
         <f t="shared" si="0"/>
         <v>7.969211453243318E-4</v>
       </c>
-      <c r="AD23">
-        <f t="shared" si="1"/>
-        <v>9.6937459744447275E-5</v>
+      <c r="AD23" s="1">
+        <f t="shared" si="5"/>
+        <v>1.5647027945955798E-4</v>
       </c>
       <c r="AE23">
         <v>0</v>
       </c>
-      <c r="AF23">
-        <f t="shared" si="2"/>
-        <v>1.384820853492104E-3</v>
+      <c r="AF23" s="1">
+        <f t="shared" si="6"/>
+        <v>2.2352897065651138E-3</v>
       </c>
       <c r="AG23" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>3.320504772184716E-7</v>
       </c>
       <c r="AH23" s="1">
@@ -3423,31 +3648,42 @@
         <f t="shared" si="9"/>
         <v>1.6602523860923581E-9</v>
       </c>
-      <c r="AN23" s="11"/>
-      <c r="AO23" s="12" t="e">
+      <c r="AM23" s="17">
+        <v>6</v>
+      </c>
+      <c r="AN23" s="17">
         <f t="shared" si="10"/>
+        <v>471.22437760150797</v>
+      </c>
+      <c r="AO23" s="17">
+        <f t="shared" si="11"/>
+        <v>6731.7768228786845</v>
+      </c>
+      <c r="AP23" s="11"/>
+      <c r="AQ23" s="12" t="e">
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AP23" s="11" t="e">
+      <c r="AR23" s="11" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS23" s="12" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT23" s="12">
+        <f t="shared" si="2"/>
+        <v>3.320504772184716E-7</v>
+      </c>
+      <c r="AU23" s="11"/>
+      <c r="AV23" s="11">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AQ23" s="12" t="e">
-        <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AR23" s="12">
-        <f t="shared" si="4"/>
-        <v>3.320504772184716E-7</v>
-      </c>
-      <c r="AS23" s="11"/>
-      <c r="AT23" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A24" s="49"/>
       <c r="B24">
         <v>1</v>
       </c>
@@ -3470,11 +3706,11 @@
         <v>33</v>
       </c>
       <c r="I24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2.894E-2</v>
       </c>
       <c r="J24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.894E-2</v>
       </c>
       <c r="K24" s="1">
@@ -3535,19 +3771,19 @@
         <f t="shared" si="0"/>
         <v>3.8437288342130877E-4</v>
       </c>
-      <c r="AD24">
-        <f t="shared" si="1"/>
-        <v>4.6755103854530141E-5</v>
+      <c r="AD24" s="1">
+        <f t="shared" si="5"/>
+        <v>7.5469113648793005E-5</v>
       </c>
       <c r="AE24">
         <v>0</v>
       </c>
-      <c r="AF24">
-        <f t="shared" si="2"/>
-        <v>6.6793005506471631E-4</v>
+      <c r="AF24" s="1">
+        <f t="shared" si="6"/>
+        <v>1.078130194982757E-3</v>
       </c>
       <c r="AG24" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1.6015536809221198E-7</v>
       </c>
       <c r="AH24" s="1">
@@ -3569,30 +3805,41 @@
         <f t="shared" si="9"/>
         <v>8.0077684046105991E-10</v>
       </c>
-      <c r="AN24" s="11"/>
-      <c r="AO24" s="12" t="e">
+      <c r="AM24" s="18">
+        <v>6</v>
+      </c>
+      <c r="AN24" s="18">
         <f t="shared" si="10"/>
+        <v>471.22437760150797</v>
+      </c>
+      <c r="AO24" s="18">
+        <f t="shared" si="11"/>
+        <v>6731.7768228786845</v>
+      </c>
+      <c r="AP24" s="11"/>
+      <c r="AQ24" s="12" t="e">
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AP24" s="11" t="e">
+      <c r="AR24" s="11" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AS24" s="12" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT24" s="12">
+        <f t="shared" si="2"/>
+        <v>1.6015536809221198E-7</v>
+      </c>
+      <c r="AU24" s="11"/>
+      <c r="AV24" s="11">
         <f t="shared" si="3"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AQ24" s="12" t="e">
-        <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AR24" s="12">
-        <f t="shared" si="4"/>
-        <v>1.6015536809221198E-7</v>
-      </c>
-      <c r="AS24" s="11"/>
-      <c r="AT24" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
@@ -3604,8 +3851,8 @@
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
     </row>
-    <row r="26" spans="1:46" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52" t="s">
+    <row r="26" spans="1:48" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="49" t="s">
         <v>81</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -3665,15 +3912,26 @@
       <c r="T26" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="Z26" s="5"/>
+      <c r="U26" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="V26" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="W26" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="AA26" s="5"/>
-      <c r="AB26" s="5"/>
+      <c r="AB26" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="AC26" s="5"/>
       <c r="AD26" s="5"/>
       <c r="AE26" s="5"/>
-    </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
+      <c r="AF26" s="5"/>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A27" s="49"/>
       <c r="B27">
         <v>1</v>
       </c>
@@ -3704,26 +3962,26 @@
         <v>3.3600000000000004E-5</v>
       </c>
       <c r="K27">
-        <f t="shared" ref="K27:K32" si="14">I27*$U$28</f>
-        <v>1.9618093457943928</v>
+        <f>I27*$V27</f>
+        <v>1.827940626717977</v>
       </c>
       <c r="L27">
-        <f t="shared" ref="L27:L32" si="15">I27*$V$28</f>
-        <v>28.025847797062756</v>
+        <f>I27*$W27</f>
+        <v>26.113437524542526</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
       <c r="N27" s="1">
-        <f t="shared" ref="N27:N32" si="16">I27*$Z$28</f>
+        <f t="shared" ref="N27:N32" si="16">I27*$AA$28</f>
         <v>16.128</v>
       </c>
       <c r="O27">
         <v>2.4000000000000001E-4</v>
       </c>
       <c r="P27" s="1">
-        <f t="shared" ref="P27:P32" si="17">I27*$AA$28</f>
-        <v>1.008</v>
+        <f t="shared" ref="P27:P32" si="17">I27*$AB27</f>
+        <v>0.40992000000000001</v>
       </c>
       <c r="Q27">
         <v>0.8</v>
@@ -3737,33 +3995,39 @@
       <c r="T27" s="17">
         <v>28</v>
       </c>
-      <c r="U27" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="V27" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="W27" s="20" t="s">
+      <c r="U27" s="17">
+        <v>4.3</v>
+      </c>
+      <c r="V27" s="17">
+        <f>(($U27/100)*(1+$AA$28*$E$43)-$X$28)/(((1+1/$W$35)*(14*10^(-6)))-(($J$43/$W$35+$F$43)*$U27/100))</f>
+        <v>272.01497421398466</v>
+      </c>
+      <c r="W27" s="17">
+        <f>$V27/$W$35</f>
+        <v>3885.9282030569234</v>
+      </c>
+      <c r="X27" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="X27" s="20" t="s">
+      <c r="Y27" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="Y27" s="20" t="s">
+      <c r="Z27" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="Z27" s="21" t="s">
+      <c r="AA27" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="AA27" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
+      <c r="AB27" s="17">
+        <f>ROUND(W27/$AO$18*100,0)</f>
+        <v>61</v>
+      </c>
+      <c r="AC27" s="51"/>
       <c r="AD27" s="1"/>
-    </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
+      <c r="AE27" s="1"/>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A28" s="49"/>
       <c r="B28">
         <v>1</v>
       </c>
@@ -3794,12 +4058,12 @@
         <v>1.1400000000000003E-5</v>
       </c>
       <c r="K28">
-        <f t="shared" si="14"/>
-        <v>0.66561388518024045</v>
+        <f>I28*$V28</f>
+        <v>0.17314941707052978</v>
       </c>
       <c r="L28">
-        <f t="shared" si="15"/>
-        <v>9.5087697882891504</v>
+        <f t="shared" ref="L28:L32" si="19">I28*$W28</f>
+        <v>2.4735631010075676</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -3813,7 +4077,7 @@
       </c>
       <c r="P28" s="1">
         <f t="shared" si="17"/>
-        <v>0.34200000000000003</v>
+        <v>3.8760000000000003E-2</v>
       </c>
       <c r="Q28">
         <v>0.4</v>
@@ -3827,35 +4091,39 @@
       <c r="T28" s="17">
         <v>0.08</v>
       </c>
-      <c r="U28" s="41">
-        <f>(($W$31/100)*(1+$Z$28*$E$43)-$W$28)/(((1+1/$V$31)*(14*10^(-6)))-(($J$43/$V$31+$F$43)*$W$31/100))</f>
-        <v>291.93591455273702</v>
-      </c>
-      <c r="V28" s="41">
-        <f>$U$28/$V$31</f>
-        <v>4170.5130650391002</v>
-      </c>
-      <c r="W28" s="23">
+      <c r="U28" s="17">
+        <v>1.8</v>
+      </c>
+      <c r="V28" s="17">
+        <f t="shared" ref="V28:V32" si="20">(($U28/100)*(1+$AA$28*$E$43)-$X$28)/(((1+1/$W$35)*(14*10^(-6)))-(($J$43/$W$35+$F$43)*$U28/100))</f>
+        <v>75.942726785320062</v>
+      </c>
+      <c r="W28" s="17">
+        <f>$V28/$W$35</f>
+        <v>1084.8960969331436</v>
+      </c>
+      <c r="X28" s="21">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="X28" s="23">
+      <c r="Y28" s="21">
         <v>1</v>
       </c>
-      <c r="Y28" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="24">
+      <c r="Z28" s="21">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="22">
         <v>2400</v>
       </c>
-      <c r="AA28" s="25">
-        <v>150</v>
-      </c>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="1"/>
+      <c r="AB28" s="17">
+        <f t="shared" ref="AB28:AB32" si="21">ROUND(W28/$AO$18*100,0)</f>
+        <v>17</v>
+      </c>
+      <c r="AC28" s="51"/>
       <c r="AD28" s="1"/>
-    </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
+      <c r="AE28" s="1"/>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A29" s="49"/>
       <c r="B29">
         <v>1</v>
       </c>
@@ -3886,12 +4154,12 @@
         <v>3.9199999999999997E-5</v>
       </c>
       <c r="K29">
-        <f t="shared" si="14"/>
-        <v>2.2887775700934583</v>
+        <f t="shared" ref="K29:K32" si="22">I29*$V29</f>
+        <v>2.5351236149918108</v>
       </c>
       <c r="L29">
-        <f t="shared" si="15"/>
-        <v>32.696822429906547</v>
+        <f t="shared" si="19"/>
+        <v>36.216051642740148</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -3905,7 +4173,7 @@
       </c>
       <c r="P29" s="1">
         <f t="shared" si="17"/>
-        <v>1.1759999999999999</v>
+        <v>0.57231999999999994</v>
       </c>
       <c r="Q29">
         <v>1</v>
@@ -3919,22 +4187,30 @@
       <c r="T29" s="17">
         <v>28</v>
       </c>
-      <c r="U29" s="42">
-        <v>175.5</v>
-      </c>
-      <c r="V29" s="43">
-        <v>2130.5</v>
-      </c>
-      <c r="X29" s="44"/>
-      <c r="Z29" s="1"/>
+      <c r="U29" s="17">
+        <v>4.8</v>
+      </c>
+      <c r="V29" s="17">
+        <f t="shared" si="20"/>
+        <v>323.35760395303708</v>
+      </c>
+      <c r="W29" s="17">
+        <f t="shared" ref="W29:W32" si="23">$V29/$W$35</f>
+        <v>4619.3943421862432</v>
+      </c>
+      <c r="Y29" s="38"/>
       <c r="AA29" s="1"/>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="1"/>
+      <c r="AB29" s="17">
+        <f t="shared" si="21"/>
+        <v>73</v>
+      </c>
+      <c r="AC29" s="51"/>
       <c r="AD29" s="1"/>
       <c r="AE29" s="1"/>
-    </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A30" s="52"/>
+      <c r="AF29" s="1"/>
+    </row>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A30" s="49"/>
       <c r="B30">
         <v>1</v>
       </c>
@@ -3965,12 +4241,12 @@
         <v>1.1400000000000003E-5</v>
       </c>
       <c r="K30">
-        <f t="shared" si="14"/>
-        <v>0.66561388518024045</v>
+        <f t="shared" si="22"/>
+        <v>0.24790115782792363</v>
       </c>
       <c r="L30">
-        <f t="shared" si="15"/>
-        <v>9.5087697882891504</v>
+        <f t="shared" si="19"/>
+        <v>3.5414451118274801</v>
       </c>
       <c r="M30">
         <v>0</v>
@@ -3984,7 +4260,7 @@
       </c>
       <c r="P30" s="1">
         <f t="shared" si="17"/>
-        <v>0.34200000000000003</v>
+        <v>5.7000000000000009E-2</v>
       </c>
       <c r="Q30">
         <v>0.5</v>
@@ -3998,21 +4274,29 @@
       <c r="T30" s="17">
         <v>0.08</v>
       </c>
-      <c r="V30" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="W30" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z30" s="1"/>
+      <c r="U30" s="17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V30" s="17">
+        <f t="shared" si="20"/>
+        <v>108.72857799470333</v>
+      </c>
+      <c r="W30" s="17">
+        <f t="shared" si="23"/>
+        <v>1553.2653999243332</v>
+      </c>
       <c r="AA30" s="1"/>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="1"/>
+      <c r="AB30" s="17">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="AC30" s="51"/>
       <c r="AD30" s="1"/>
       <c r="AE30" s="1"/>
-    </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
+      <c r="AF30" s="1"/>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A31" s="49"/>
       <c r="B31">
         <v>1</v>
       </c>
@@ -4043,12 +4327,12 @@
         <v>2.0000000000000002E-7</v>
       </c>
       <c r="K31">
-        <f t="shared" si="14"/>
-        <v>1.1677436582109482E-2</v>
+        <f t="shared" si="22"/>
+        <v>4.3491431197881332E-3</v>
       </c>
       <c r="L31">
-        <f t="shared" si="15"/>
-        <v>0.16682052260156402</v>
+        <f t="shared" si="19"/>
+        <v>6.2130615996973337E-2</v>
       </c>
       <c r="M31">
         <v>0</v>
@@ -4062,7 +4346,7 @@
       </c>
       <c r="P31" s="1">
         <f t="shared" si="17"/>
-        <v>6.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="Q31">
         <v>0.5</v>
@@ -4076,24 +4360,34 @@
       <c r="T31" s="17">
         <v>0.08</v>
       </c>
-      <c r="V31" s="18">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="W31" s="18">
-        <v>4.5</v>
-      </c>
-      <c r="AM31" s="53" t="s">
+      <c r="U31" s="17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V31" s="17">
+        <f t="shared" si="20"/>
+        <v>108.72857799470333</v>
+      </c>
+      <c r="W31" s="17">
+        <f t="shared" si="23"/>
+        <v>1553.2653999243332</v>
+      </c>
+      <c r="AB31" s="17">
+        <f t="shared" si="21"/>
+        <v>25</v>
+      </c>
+      <c r="AC31" s="51"/>
+      <c r="AP31" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="AN31" s="11" t="s">
+      <c r="AQ31" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AO31" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
+      <c r="AR31" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A32" s="49"/>
       <c r="B32">
         <v>1</v>
       </c>
@@ -4124,12 +4418,12 @@
         <v>3.1920000000000006E-5</v>
       </c>
       <c r="K32">
-        <f t="shared" si="14"/>
-        <v>1.8637188785046734</v>
+        <f t="shared" si="22"/>
+        <v>2.277715012925035</v>
       </c>
       <c r="L32">
-        <f t="shared" si="15"/>
-        <v>26.62455540720962</v>
+        <f t="shared" si="19"/>
+        <v>32.538785898929063</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -4143,7 +4437,7 @@
       </c>
       <c r="P32" s="1">
         <f t="shared" si="17"/>
-        <v>0.95760000000000012</v>
+        <v>0.51072000000000006</v>
       </c>
       <c r="Q32">
         <v>1.2</v>
@@ -4157,58 +4451,92 @@
       <c r="T32" s="18">
         <v>28</v>
       </c>
-      <c r="AM32" s="53"/>
-      <c r="AN32" s="11" t="s">
+      <c r="U32" s="18">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="V32" s="18">
+        <f t="shared" si="20"/>
+        <v>356.78493310229237</v>
+      </c>
+      <c r="W32" s="18">
+        <f t="shared" si="23"/>
+        <v>5096.9276157470331</v>
+      </c>
+      <c r="AB32" s="18">
+        <f t="shared" si="21"/>
+        <v>80</v>
+      </c>
+      <c r="AC32" s="51"/>
+      <c r="AP32" s="46"/>
+      <c r="AQ32" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AO32" s="11">
+      <c r="AR32" s="11">
         <v>0.106</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="AM33" s="53"/>
-      <c r="AN33" s="11" t="s">
+      <c r="AM33" s="46"/>
+      <c r="AN33" s="46"/>
+      <c r="AO33" s="46"/>
+      <c r="AP33" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AO33" s="11">
+      <c r="AQ33" s="11">
         <v>1.28</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="AM34" s="53"/>
-      <c r="AN34" s="11" t="s">
+      <c r="W34" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="X34" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM34" s="46"/>
+      <c r="AN34" s="46"/>
+      <c r="AO34" s="46"/>
+      <c r="AP34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AO34" s="11">
+      <c r="AQ34" s="11">
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="AM35" s="53"/>
-      <c r="AN35" s="11" t="s">
+      <c r="W35" s="18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X35" s="18"/>
+      <c r="AM35" s="46"/>
+      <c r="AN35" s="46"/>
+      <c r="AO35" s="46"/>
+      <c r="AP35" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="AO35" s="11">
+      <c r="AQ35" s="11">
         <f>210*3600*24/12</f>
         <v>1512000</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="F36" s="1"/>
       <c r="AM36" s="11"/>
-      <c r="AN36" s="11" t="s">
+      <c r="AN36" s="11"/>
+      <c r="AO36" s="11"/>
+      <c r="AP36" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="AO36" s="11">
+      <c r="AQ36" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A37" s="52" t="s">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A37" s="49" t="s">
         <v>82</v>
       </c>
       <c r="B37" s="9" t="s">
@@ -4250,16 +4578,18 @@
       <c r="R37" s="3"/>
       <c r="S37" s="2"/>
       <c r="AM37" s="13"/>
-      <c r="AN37" s="11" t="s">
+      <c r="AN37" s="13"/>
+      <c r="AO37" s="13"/>
+      <c r="AP37" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="AO37" s="11">
+      <c r="AQ37" s="11">
         <f>1/59</f>
         <v>1.6949152542372881E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A38" s="52"/>
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A38" s="49"/>
       <c r="B38">
         <v>1</v>
       </c>
@@ -4269,41 +4599,43 @@
       <c r="D38" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="44">
-        <f>SUM($K$39,$I$27:$I$32,$AI$17:$AI$24)*Z28</f>
+      <c r="E38" s="38">
+        <f>SUM($K$39,$I$27:$I$32,$AI$17:$AI$24)*AA28</f>
         <v>124.22506218605774</v>
       </c>
-      <c r="F38" s="44">
-        <f>SUM($K$39,$I$27:$I$32,$AI$17:$AI$24)*U28</f>
-        <v>15.110732141523915</v>
-      </c>
-      <c r="G38" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="H38" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="I38" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="J38" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="K38" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="L38" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="M38" s="44" t="s">
+      <c r="F38" s="38">
+        <f>SUM(K27:K32,F39,AD17:AD24)</f>
+        <v>15.725750930581162</v>
+      </c>
+      <c r="G38" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="H38" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="I38" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="J38" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="K38" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="L38" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="M38" s="38" t="s">
         <v>32</v>
       </c>
       <c r="AM38" s="14"/>
-      <c r="AN38" s="11"/>
-      <c r="AO38" s="11"/>
-    </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A39" s="52"/>
+      <c r="AN38" s="14"/>
+      <c r="AO38" s="14"/>
+      <c r="AP38" s="11"/>
+      <c r="AQ38" s="11"/>
+    </row>
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A39" s="49"/>
       <c r="B39">
         <v>1</v>
       </c>
@@ -4313,49 +4645,49 @@
       <c r="D39" t="s">
         <v>78</v>
       </c>
-      <c r="E39" s="44">
+      <c r="E39" s="38">
         <f>E40*$K$39</f>
         <v>56.465937357298984</v>
       </c>
-      <c r="F39" s="44">
+      <c r="F39" s="38">
         <f>F40*$K$39</f>
-        <v>30.911884999170226</v>
-      </c>
-      <c r="G39" s="44">
-        <f t="shared" ref="G39" si="19">G40*$K$39</f>
-        <v>26.420414529205321</v>
-      </c>
-      <c r="H39" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="I39" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="J39" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="K39" s="44">
+        <v>7.7277871788939576</v>
+      </c>
+      <c r="G39" s="38">
+        <f>G40*$K$39</f>
+        <v>6.6049463067469727</v>
+      </c>
+      <c r="H39" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="I39" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="J39" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="K39" s="38">
         <f>SUM(AI17:AI24,I27:I32)/$O$40</f>
         <v>2.3527473898874576E-2</v>
       </c>
-      <c r="L39" s="44">
-        <f>K39*$W$28</f>
+      <c r="L39" s="38">
+        <f>K39*$X$28</f>
         <v>1.1763736949437288E-4</v>
       </c>
-      <c r="M39" s="44">
+      <c r="M39" s="38">
         <f>M40*$K$39</f>
-        <v>0.94109895595498305</v>
-      </c>
-      <c r="O39" s="26" t="s">
+        <v>0.11763736949437288</v>
+      </c>
+      <c r="O39" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="P39" s="26" t="s">
+      <c r="P39" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="Q39" s="26" t="s">
+      <c r="Q39" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="R39" s="53" t="s">
+      <c r="R39" s="50" t="s">
         <v>56</v>
       </c>
       <c r="S39" s="11" t="s">
@@ -4365,28 +4697,30 @@
         <v>2.6499999999999999E-8</v>
       </c>
       <c r="AM39" s="14"/>
-      <c r="AN39" s="11"/>
-      <c r="AO39" s="11"/>
-    </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="E40" s="27">
+      <c r="AN39" s="14"/>
+      <c r="AO39" s="14"/>
+      <c r="AP39" s="11"/>
+      <c r="AQ39" s="11"/>
+    </row>
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="E40" s="24">
         <v>2400</v>
       </c>
-      <c r="F40" s="32">
-        <f>(($Q$40/100)*(1+$E$40*$E$43)-$W$28)/((1+1/$P$40)*(14*10^-6-$J$43*$Q$40/100))</f>
-        <v>1313.8633213253243</v>
-      </c>
-      <c r="G40" s="32">
+      <c r="F40" s="29">
+        <f>(($Q$40/100)*(1+$E$40*$E$43)-$X$28)/((1+1/$P$40)*(14*10^-6-$J$43*$Q$40/100))</f>
+        <v>328.45800667378967</v>
+      </c>
+      <c r="G40" s="29">
         <f>F40/$P$40</f>
-        <v>1122.9601036968584</v>
-      </c>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="29">
-        <v>40</v>
+        <v>280.73333903742707</v>
+      </c>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="26">
+        <v>5</v>
       </c>
       <c r="O40" s="18">
         <v>1.2</v>
@@ -4395,9 +4729,9 @@
         <v>1.17</v>
       </c>
       <c r="Q40" s="18">
-        <v>3</v>
-      </c>
-      <c r="R40" s="53"/>
+        <v>1.2</v>
+      </c>
+      <c r="R40" s="50"/>
       <c r="S40" s="11" t="s">
         <v>58</v>
       </c>
@@ -4407,12 +4741,14 @@
       <c r="AM40" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="AN40" s="11"/>
-      <c r="AO40" s="11"/>
-    </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AN40" s="14"/>
+      <c r="AO40" s="14"/>
+      <c r="AP40" s="11"/>
+      <c r="AQ40" s="11"/>
+    </row>
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="F41" s="1"/>
-      <c r="R41" s="53"/>
+      <c r="R41" s="50"/>
       <c r="S41" s="11" t="s">
         <v>59</v>
       </c>
@@ -4422,15 +4758,17 @@
       <c r="AM41" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="AN41" s="11"/>
-      <c r="AO41" s="11"/>
-    </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="D42" s="40" t="s">
+      <c r="AN41" s="15"/>
+      <c r="AO41" s="15"/>
+      <c r="AP41" s="11"/>
+      <c r="AQ41" s="11"/>
+    </row>
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="D42" s="37" t="s">
         <v>134</v>
       </c>
       <c r="F42" s="1"/>
-      <c r="R42" s="53"/>
+      <c r="R42" s="50"/>
       <c r="S42" s="11" t="s">
         <v>60</v>
       </c>
@@ -4438,26 +4776,28 @@
         <v>0.8</v>
       </c>
       <c r="AM42" s="15"/>
-      <c r="AN42" s="11"/>
-      <c r="AO42" s="11"/>
-    </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="D43" s="30" t="s">
+      <c r="AN42" s="15"/>
+      <c r="AO42" s="15"/>
+      <c r="AP42" s="11"/>
+      <c r="AQ42" s="11"/>
+    </row>
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="D43" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="E43" s="30">
+      <c r="E43" s="27">
         <f xml:space="preserve"> (0.000001*12) / 0.42</f>
         <v>2.8571428571428574E-5</v>
       </c>
-      <c r="F43" s="31">
+      <c r="F43" s="28">
         <f>( 0.000001*14) / 0.145</f>
         <v>9.6551724137931033E-5</v>
       </c>
-      <c r="J43" s="31">
+      <c r="J43" s="28">
         <f>( 0.000001*14) / 0.145</f>
         <v>9.6551724137931033E-5</v>
       </c>
-      <c r="R43" s="53"/>
+      <c r="R43" s="50"/>
       <c r="S43" s="11" t="s">
         <v>61</v>
       </c>
@@ -4468,20 +4808,22 @@
       <c r="AM43" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="AN43" s="11"/>
-      <c r="AO43" s="11"/>
-    </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="D44" s="30" t="s">
+      <c r="AN43" s="14"/>
+      <c r="AO43" s="14"/>
+      <c r="AP43" s="11"/>
+      <c r="AQ43" s="11"/>
+    </row>
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="D44" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="30">
+      <c r="E44" s="27">
         <f>E38*E43</f>
         <v>3.5492874910302216E-3</v>
       </c>
-      <c r="F44" s="31">
+      <c r="F44" s="28">
         <f>F38*F43</f>
-        <v>1.4589672412505849E-3</v>
+        <v>1.5183483657112845E-3</v>
       </c>
       <c r="R44" s="15"/>
       <c r="S44" s="13" t="s">
@@ -4492,10 +4834,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="R39:R43"/>
-    <mergeCell ref="AM31:AM35"/>
     <mergeCell ref="A3:A12"/>
     <mergeCell ref="A16:A24"/>
     <mergeCell ref="A26:A32"/>
@@ -4507,10 +4848,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U63"/>
+  <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4527,7 +4868,7 @@
       <c r="A2" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="30" t="s">
         <v>88</v>
       </c>
       <c r="C2" t="s">
@@ -4592,7 +4933,7 @@
       <c r="A3">
         <v>9</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="31">
         <v>38778</v>
       </c>
       <c r="C3">
@@ -4654,7 +4995,7 @@
       <c r="A4">
         <v>9</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="31">
         <v>38778</v>
       </c>
       <c r="C4">
@@ -4713,7 +5054,7 @@
       <c r="A5">
         <v>9</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="31">
         <v>38778</v>
       </c>
       <c r="C5">
@@ -4772,7 +5113,7 @@
       <c r="A6">
         <v>9</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="31">
         <v>38778</v>
       </c>
       <c r="C6">
@@ -4828,7 +5169,7 @@
       <c r="A7">
         <v>9</v>
       </c>
-      <c r="B7" s="34">
+      <c r="B7" s="31">
         <v>38778</v>
       </c>
       <c r="C7">
@@ -4887,7 +5228,7 @@
       <c r="A8">
         <v>9</v>
       </c>
-      <c r="B8" s="34">
+      <c r="B8" s="31">
         <v>38778</v>
       </c>
       <c r="C8">
@@ -4949,7 +5290,7 @@
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9" s="34">
+      <c r="B9" s="31">
         <v>38778</v>
       </c>
       <c r="C9">
@@ -5008,7 +5349,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="34">
+      <c r="B10" s="31">
         <v>38778</v>
       </c>
       <c r="C10">
@@ -5067,7 +5408,7 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="31">
         <v>38778</v>
       </c>
       <c r="C11">
@@ -5123,7 +5464,7 @@
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="34">
+      <c r="B12" s="31">
         <v>38778</v>
       </c>
       <c r="C12">
@@ -5182,7 +5523,7 @@
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="34">
+      <c r="B13" s="31">
         <v>38778</v>
       </c>
       <c r="C13">
@@ -5244,7 +5585,7 @@
       <c r="A14">
         <v>9</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="31">
         <v>38778</v>
       </c>
       <c r="C14">
@@ -5303,7 +5644,7 @@
       <c r="A15">
         <v>9</v>
       </c>
-      <c r="B15" s="34">
+      <c r="B15" s="31">
         <v>38778</v>
       </c>
       <c r="C15">
@@ -5362,7 +5703,7 @@
       <c r="A16">
         <v>9</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="31">
         <v>38778</v>
       </c>
       <c r="C16">
@@ -5421,7 +5762,7 @@
       <c r="A17">
         <v>9</v>
       </c>
-      <c r="B17" s="34">
+      <c r="B17" s="31">
         <v>38778</v>
       </c>
       <c r="C17">
@@ -5477,24 +5818,24 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I19" s="35" t="s">
+      <c r="I19" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="J19" s="36">
+      <c r="J19" s="33">
         <f>SUM(J3:K17)</f>
         <v>1.04674</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="J20" s="38">
+      <c r="J20" s="35">
         <f>(SUMPRODUCT(P3:P17,J3:J17)+SUMPRODUCT(K3:K17,Q3:Q17))/J19</f>
         <v>3.8773662250209906</v>
       </c>
     </row>
-    <row r="22" spans="1:21" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>117</v>
       </c>
@@ -5547,7 +5888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>124</v>
       </c>
@@ -5591,7 +5932,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>131</v>
       </c>
@@ -5700,7 +6041,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>168</v>
       </c>
@@ -5715,9 +6056,255 @@
         <v>170</v>
       </c>
     </row>
+    <row r="66" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>190</v>
+      </c>
+      <c r="B67" t="s">
+        <v>191</v>
+      </c>
+      <c r="F67" t="s">
+        <v>201</v>
+      </c>
+      <c r="G67" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="30">
+        <v>41982</v>
+      </c>
+      <c r="B68">
+        <v>2.9</v>
+      </c>
+      <c r="C68" t="s">
+        <v>192</v>
+      </c>
+      <c r="F68" t="s">
+        <v>202</v>
+      </c>
+      <c r="G68" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>193</v>
+      </c>
+      <c r="B70" t="s">
+        <v>194</v>
+      </c>
+      <c r="C70" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>196</v>
+      </c>
+      <c r="B71">
+        <v>2.2870125000000003</v>
+      </c>
+      <c r="C71">
+        <v>0.7309330444956722</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="B72">
+        <v>2.2870125000000003</v>
+      </c>
+      <c r="C72">
+        <v>0.7309330444956722</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1</v>
+      </c>
+      <c r="B73">
+        <v>1.75</v>
+      </c>
+      <c r="C73">
+        <v>0.20952326839756921</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>2</v>
+      </c>
+      <c r="B74">
+        <v>2.2815250000000002</v>
+      </c>
+      <c r="C74">
+        <v>0.20010489540904686</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>3.92</v>
+      </c>
+      <c r="C75" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>197</v>
+      </c>
+      <c r="B76">
+        <v>1.0091249999999998</v>
+      </c>
+      <c r="C76">
+        <v>0.47786590430789283</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>0</v>
+      </c>
+      <c r="B77">
+        <v>1.0091249999999998</v>
+      </c>
+      <c r="C77">
+        <v>0.47786590430789283</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>0</v>
+      </c>
+      <c r="B78">
+        <v>1.0091249999999998</v>
+      </c>
+      <c r="C78">
+        <v>0.47786590430789283</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>198</v>
+      </c>
+      <c r="B79">
+        <v>4.8106111111111112</v>
+      </c>
+      <c r="C79">
+        <v>0.51639141548532097</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>199</v>
+      </c>
+      <c r="B80">
+        <v>4.9147749999999997</v>
+      </c>
+      <c r="C80">
+        <v>0.98298377868949161</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>3</v>
+      </c>
+      <c r="B81">
+        <v>4.6097666666666663</v>
+      </c>
+      <c r="C81">
+        <v>0.94403663241070213</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>4</v>
+      </c>
+      <c r="B82">
+        <v>5.8297999999999996</v>
+      </c>
+      <c r="C82" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>200</v>
+      </c>
+      <c r="B83">
+        <v>4.78085</v>
+      </c>
+      <c r="C83">
+        <v>0.34847466247149217</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>1</v>
+      </c>
+      <c r="B84">
+        <v>4.3347250000000006</v>
+      </c>
+      <c r="C84">
+        <v>9.8384801502363659E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2</v>
+      </c>
+      <c r="B85">
+        <v>4.790375</v>
+      </c>
+      <c r="C85">
+        <v>0.16446041823692564</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>3</v>
+      </c>
+      <c r="B86">
+        <v>5.0953749999999998</v>
+      </c>
+      <c r="C86">
+        <v>0.11109150507579962</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>4</v>
+      </c>
+      <c r="B87">
+        <v>5.0250000000000004</v>
+      </c>
+      <c r="C87">
+        <v>0.34648232278139673</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>188</v>
+      </c>
+      <c r="B89">
+        <v>1.1827218811602722</v>
+      </c>
+      <c r="C89">
+        <v>0.11366340365867296</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5731,12 +6318,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>131</v>
       </c>
@@ -5746,7 +6333,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>141</v>
       </c>
@@ -5839,15 +6426,15 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="48" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="49" t="s">
+    <row r="15" spans="1:12" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="50">
+      <c r="D15" s="44">
         <f>D13/D12</f>
         <v>6.6225165562913912E-2</v>
       </c>
-      <c r="G15" s="48" t="s">
+      <c r="G15" s="42" t="s">
         <v>150</v>
       </c>
     </row>
@@ -5857,17 +6444,17 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="45" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="45" t="s">
+      <c r="G18" s="39" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="45" t="s">
+      <c r="G19" s="39" t="s">
         <v>152</v>
       </c>
     </row>
@@ -5911,7 +6498,7 @@
         <f>A2*476</f>
         <v>0</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="38">
         <f>IF(A2&lt;1.55,4.4,5.35*A2^-0.442)</f>
         <v>4.4000000000000004</v>
       </c>
@@ -5924,7 +6511,7 @@
         <f t="shared" ref="B3:B16" si="0">A3*476</f>
         <v>476</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="38">
         <f t="shared" ref="C3:C4" si="1">IF(A3&lt;1.55,4.4,5.35*A3^-0.442)</f>
         <v>4.4000000000000004</v>
       </c>
@@ -5937,7 +6524,7 @@
         <f t="shared" si="0"/>
         <v>952</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="38">
         <f t="shared" si="1"/>
         <v>3.9382068562998769</v>
       </c>
@@ -5950,7 +6537,7 @@
         <f t="shared" si="0"/>
         <v>1428</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="38">
         <f t="shared" ref="C5:C16" si="2">IF(A5&lt;1.55,4.4,5.35*A5^-0.442)</f>
         <v>3.2920482166369851</v>
       </c>
@@ -5963,7 +6550,7 @@
         <f t="shared" si="0"/>
         <v>1904</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="38">
         <f t="shared" si="2"/>
         <v>2.898966961309787</v>
       </c>
@@ -5976,7 +6563,7 @@
         <f t="shared" si="0"/>
         <v>2380</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="38">
         <f t="shared" si="2"/>
         <v>2.6266913270069852</v>
       </c>
@@ -5989,7 +6576,7 @@
         <f t="shared" si="0"/>
         <v>2856</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="38">
         <f t="shared" si="2"/>
         <v>2.4233209080429079</v>
       </c>
@@ -6002,7 +6589,7 @@
         <f t="shared" si="0"/>
         <v>3332</v>
       </c>
-      <c r="C9" s="44">
+      <c r="C9" s="38">
         <f t="shared" si="2"/>
         <v>2.2637082224491012</v>
       </c>
@@ -6015,7 +6602,7 @@
         <f t="shared" si="0"/>
         <v>3808</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="38">
         <f t="shared" si="2"/>
         <v>2.1339685164891629</v>
       </c>
@@ -6028,7 +6615,7 @@
         <f t="shared" si="0"/>
         <v>4284</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="38">
         <f t="shared" si="2"/>
         <v>2.0257161608715433</v>
       </c>
@@ -6041,7 +6628,7 @@
         <f t="shared" si="0"/>
         <v>4760</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="38">
         <f t="shared" si="2"/>
         <v>1.9335427651219308</v>
       </c>
@@ -6054,7 +6641,7 @@
         <f t="shared" si="0"/>
         <v>5236</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="38">
         <f t="shared" si="2"/>
         <v>1.8537800974717134</v>
       </c>
@@ -6067,7 +6654,7 @@
         <f t="shared" si="0"/>
         <v>5712</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="38">
         <f t="shared" si="2"/>
         <v>1.7838390682372756</v>
       </c>
@@ -6080,7 +6667,7 @@
         <f t="shared" si="0"/>
         <v>6188</v>
       </c>
-      <c r="C15" s="44">
+      <c r="C15" s="38">
         <f t="shared" si="2"/>
         <v>1.721832180171422</v>
       </c>
@@ -6093,7 +6680,7 @@
         <f t="shared" si="0"/>
         <v>6664</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="38">
         <f t="shared" si="2"/>
         <v>1.6663460266002725</v>
       </c>
@@ -6101,4 +6688,455 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>34.6</v>
+      </c>
+      <c r="D5">
+        <v>140</v>
+      </c>
+      <c r="E5">
+        <v>0.97</v>
+      </c>
+      <c r="F5" s="38">
+        <f>D5/C5*10</f>
+        <v>40.462427745664733</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="I5" s="38">
+        <f>G5/D5*1000</f>
+        <v>107.14285714285714</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <v>90</v>
+      </c>
+      <c r="E6">
+        <v>0.77</v>
+      </c>
+      <c r="F6" s="38">
+        <f t="shared" ref="F6:F17" si="0">D6/C6*10</f>
+        <v>26.470588235294116</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="I6" s="38">
+        <f t="shared" ref="I6:I19" si="1">G6/D6*1000</f>
+        <v>88.888888888888886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7">
+        <v>22.8</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <v>0.47</v>
+      </c>
+      <c r="F7" s="38">
+        <f t="shared" si="0"/>
+        <v>21.929824561403507</v>
+      </c>
+      <c r="G7">
+        <v>3.5</v>
+      </c>
+      <c r="I7" s="38">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>0.34</v>
+      </c>
+      <c r="F8" s="38">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>2.5</v>
+      </c>
+      <c r="I8" s="38">
+        <f t="shared" si="1"/>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>123</v>
+      </c>
+      <c r="E9">
+        <v>0.6</v>
+      </c>
+      <c r="F9" s="38">
+        <f t="shared" si="0"/>
+        <v>205</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="38">
+        <f t="shared" si="1"/>
+        <v>4.0650406504065044</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>95</v>
+      </c>
+      <c r="E10">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F10" s="38">
+        <f t="shared" si="0"/>
+        <v>190</v>
+      </c>
+      <c r="G10">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="38">
+        <f t="shared" si="1"/>
+        <v>2.1052631578947367</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>73</v>
+      </c>
+      <c r="E11">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F11" s="38">
+        <f t="shared" si="0"/>
+        <v>182.5</v>
+      </c>
+      <c r="G11">
+        <v>0.15</v>
+      </c>
+      <c r="I11" s="38">
+        <f t="shared" si="1"/>
+        <v>2.054794520547945</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>58</v>
+      </c>
+      <c r="E12">
+        <v>0.43</v>
+      </c>
+      <c r="F12" s="38">
+        <f t="shared" si="0"/>
+        <v>290</v>
+      </c>
+      <c r="G12">
+        <v>1.5</v>
+      </c>
+      <c r="I12" s="38">
+        <f t="shared" si="1"/>
+        <v>25.862068965517242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13">
+        <v>0.8</v>
+      </c>
+      <c r="D13">
+        <v>32</v>
+      </c>
+      <c r="E13">
+        <v>0.09</v>
+      </c>
+      <c r="F13" s="38">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G13">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="38">
+        <f t="shared" si="1"/>
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>160</v>
+      </c>
+      <c r="E14">
+        <v>0.43</v>
+      </c>
+      <c r="F14" s="38">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="G14">
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="38">
+        <f t="shared" si="1"/>
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>152</v>
+      </c>
+      <c r="E15">
+        <v>0.32</v>
+      </c>
+      <c r="F15" s="38">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
+      <c r="G15">
+        <v>0.15</v>
+      </c>
+      <c r="I15" s="38">
+        <f t="shared" si="1"/>
+        <v>0.98684210526315796</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16">
+        <v>2.5</v>
+      </c>
+      <c r="D16">
+        <v>109</v>
+      </c>
+      <c r="E16">
+        <v>0.26</v>
+      </c>
+      <c r="F16" s="38">
+        <f t="shared" si="0"/>
+        <v>436</v>
+      </c>
+      <c r="G16">
+        <v>0.1</v>
+      </c>
+      <c r="I16" s="38">
+        <f t="shared" si="1"/>
+        <v>0.91743119266055051</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>74</v>
+      </c>
+      <c r="E17">
+        <v>0.31</v>
+      </c>
+      <c r="F17" s="38">
+        <f t="shared" si="0"/>
+        <v>740</v>
+      </c>
+      <c r="G17">
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="38">
+        <f t="shared" si="1"/>
+        <v>1.3513513513513513</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19">
+        <f>0.5*1000</f>
+        <v>500</v>
+      </c>
+      <c r="E19">
+        <f>0.01*1000</f>
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>2.5</v>
+      </c>
+      <c r="I19" s="38">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Correction of root mass input.
</commit_message>
<xml_diff>
--- a/branches/develop/fspmwheat/inputs/Generate_inputs.xlsx
+++ b/branches/develop/fspmwheat/inputs/Generate_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320"/>
   </bookViews>
   <sheets>
     <sheet name="INPUTS_tillering" sheetId="17" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="158">
   <si>
     <t>plant</t>
   </si>
@@ -678,6 +678,9 @@
   </si>
   <si>
     <t>SAM</t>
+  </si>
+  <si>
+    <t>Chaff</t>
   </si>
 </sst>
 </file>
@@ -1535,8 +1538,8 @@
   </sheetPr>
   <dimension ref="A1:AY66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" topLeftCell="P17" workbookViewId="0">
+      <selection activeCell="AC50" sqref="AC50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8075,15 +8078,15 @@
       </c>
       <c r="E49" s="28">
         <f>E50*$K$49</f>
-        <v>156.27632387713228</v>
+        <v>157.02970067046741</v>
       </c>
       <c r="F49" s="28">
         <f>F50*$K$49</f>
-        <v>12.615473855175905</v>
+        <v>7.8369089556621496</v>
       </c>
       <c r="G49" s="28">
         <f>G50*$K$49</f>
-        <v>10.782456286475133</v>
+        <v>15.673817911324299</v>
       </c>
       <c r="H49" s="28" t="s">
         <v>32</v>
@@ -8096,15 +8099,15 @@
       </c>
       <c r="K49" s="1">
         <f>$P$55/$O$50/(1+$E$50*$E$53+$F$50*$F$53+$G$50*$G$53)</f>
-        <v>3.5422633412149983E-2</v>
+        <v>3.559339881863928E-2</v>
       </c>
       <c r="L49" s="28">
         <f>K49*$Y$38</f>
-        <v>1.7711316706074993E-4</v>
+        <v>1.779669940931964E-4</v>
       </c>
       <c r="M49" s="28">
         <f>M50*$K$49</f>
-        <v>0.17711316706074992</v>
+        <v>0.17796699409319638</v>
       </c>
       <c r="N49" s="76" t="s">
         <v>134</v>
@@ -8142,11 +8145,11 @@
       </c>
       <c r="F50" s="58">
         <f>(($Q$50/100)*(1+$E$50*$E$53)-$Y$38)/((1+1/$P$50)*(14*10^-6-$J$53*$Q$50/100))</f>
-        <v>356.14161455451784</v>
+        <v>220.17871896960222</v>
       </c>
       <c r="G50" s="58">
         <f>F50/$P$50</f>
-        <v>304.39454235428877</v>
+        <v>440.35743793920443</v>
       </c>
       <c r="H50" s="21"/>
       <c r="I50" s="21"/>
@@ -8158,15 +8161,18 @@
       </c>
       <c r="N50" s="77">
         <f>SUM(AJ5:AJ12,J37:J42)/K49</f>
-        <v>0.56778273705800308</v>
+        <v>0.56505870245862833</v>
       </c>
       <c r="O50" s="16">
+        <f>INPUTS!O28</f>
         <v>0.8</v>
       </c>
       <c r="P50" s="16">
-        <v>1.17</v>
+        <f>INPUTS!P28</f>
+        <v>0.5</v>
       </c>
       <c r="Q50" s="16">
+        <f>INPUTS!Q28</f>
         <v>1.2</v>
       </c>
       <c r="R50" s="95"/>
@@ -8219,9 +8225,9 @@
       <c r="O52" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="P52" s="69">
-        <f>K49+SUM(J37:J42)+SUM(AJ5:AJ12)</f>
-        <v>5.553499316470277E-2</v>
+      <c r="P52" s="36">
+        <f>K49+SUM(J37:J42)+SUM(AJ5:AJ34)</f>
+        <v>5.660205295951682E-2</v>
       </c>
       <c r="R52" s="95"/>
       <c r="S52" s="9" t="s">
@@ -8546,7 +8552,7 @@
       </c>
       <c r="P60" s="39">
         <f>1-$K$49/$P$56</f>
-        <v>0.15387329166350705</v>
+        <v>0.14979428461709776</v>
       </c>
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.25">
@@ -8658,7 +8664,7 @@
       </c>
       <c r="P62" s="39">
         <f>1-$K$49/($P$56+1/(1+N50)*P54)</f>
-        <v>0.15387329166350705</v>
+        <v>0.14979428461709776</v>
       </c>
     </row>
     <row r="64" spans="1:45" x14ac:dyDescent="0.25">
@@ -8709,8 +8715,8 @@
   </sheetPr>
   <dimension ref="A1:AY44"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15:U20"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11232,15 +11238,15 @@
       </c>
       <c r="E27" s="28">
         <f>E28*$K$27</f>
-        <v>148.50745811735956</v>
+        <v>149.22338276804928</v>
       </c>
       <c r="F27" s="28">
         <f>F28*$K$27</f>
-        <v>11.988328805655543</v>
+        <v>7.4473176718540657</v>
       </c>
       <c r="G27" s="28">
         <f>G28*$K$27</f>
-        <v>10.246434876628671</v>
+        <v>14.894635343708131</v>
       </c>
       <c r="H27" s="28" t="s">
         <v>32</v>
@@ -11253,15 +11259,15 @@
       </c>
       <c r="K27" s="1">
         <f>$P$33/$O$28/(1+$E$28*$E$31+$F$28*$F$31+$G$28*$G$31)</f>
-        <v>3.3661690506601498E-2</v>
+        <v>3.3823966760757836E-2</v>
       </c>
       <c r="L27" s="28">
         <f>K27*$Y$16</f>
-        <v>1.683084525330075E-4</v>
+        <v>1.6911983380378919E-4</v>
       </c>
       <c r="M27" s="28">
         <f>M28*$K$27</f>
-        <v>0.1683084525330075</v>
+        <v>0.16911983380378917</v>
       </c>
       <c r="N27" s="76" t="s">
         <v>134</v>
@@ -11299,11 +11305,11 @@
       </c>
       <c r="F28" s="58">
         <f>(($Q$28/100)*(1+$E$28*$E$31)-$Y$16)/((1+1/$P$28)*(14*10^-6-$J$31*$Q$28/100))</f>
-        <v>356.14161455451784</v>
+        <v>220.17871896960222</v>
       </c>
       <c r="G28" s="58">
         <f>F28/$P$28</f>
-        <v>304.39454235428877</v>
+        <v>440.35743793920443</v>
       </c>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
@@ -11315,13 +11321,13 @@
       </c>
       <c r="N28" s="77">
         <f>SUM(AJ5:AJ12,J15:J20)/K27</f>
-        <v>0.5997958798894254</v>
+        <v>0.59691825677279609</v>
       </c>
       <c r="O28" s="16">
         <v>0.8</v>
       </c>
       <c r="P28" s="16">
-        <v>1.17</v>
+        <v>0.5</v>
       </c>
       <c r="Q28" s="16">
         <v>1.2</v>
@@ -11378,7 +11384,7 @@
       </c>
       <c r="P30" s="69">
         <f>K27+SUM(J15:J20)+SUM(AJ5:AJ12)</f>
-        <v>5.3851833782574056E-2</v>
+        <v>5.4014110036730394E-2</v>
       </c>
       <c r="R30" s="95"/>
       <c r="S30" s="9" t="s">
@@ -11500,7 +11506,7 @@
       </c>
       <c r="P34" s="36">
         <f>K27+E27*E31+F27*F31+G27*G31</f>
-        <v>3.9783273799241313E-2</v>
+        <v>3.978327379924132E-2</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -11609,7 +11615,7 @@
       </c>
       <c r="P38" s="39">
         <f>1-$K$27/$P$34</f>
-        <v>0.15387329166350705</v>
+        <v>0.14979428461709776</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
@@ -11627,7 +11633,7 @@
       </c>
       <c r="P40" s="39">
         <f>1-$K$27/($P$34+1/(1+N28)*P32)</f>
-        <v>0.15387329166350705</v>
+        <v>0.14979428461709776</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
@@ -17195,10 +17201,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17306,7 +17312,7 @@
         <v>8</v>
       </c>
       <c r="I6" s="28">
-        <f t="shared" ref="I6:I19" si="1">G6/D6*1000</f>
+        <f t="shared" ref="I6:I20" si="1">G6/D6*1000</f>
         <v>88.888888888888886</v>
       </c>
     </row>
@@ -17620,20 +17626,41 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>210</v>
+      </c>
+      <c r="E19">
+        <v>1.01</v>
+      </c>
+      <c r="G19">
+        <v>15</v>
+      </c>
+      <c r="I19" s="28">
+        <f t="shared" si="1"/>
+        <v>71.428571428571431</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <f>0.5*1000</f>
         <v>500</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <f>0.01*1000</f>
         <v>10</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>2.5</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I20" s="28">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>

</xml_diff>